<commit_message>
a bunch of chagnes, amazing happens
</commit_message>
<xml_diff>
--- a/templates/cpr1000/check_record.xlsx
+++ b/templates/cpr1000/check_record.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/churui/Projects/doc-server/templates/cpr1000/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\docServer\templates\cpr1000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="27240" windowHeight="14895" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>文件检查问题解决单</t>
     <phoneticPr fontId="3"/>
@@ -221,12 +221,16 @@
     <t>${pages}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>${project}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -614,6 +618,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -634,12 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -652,6 +656,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -923,72 +930,72 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:J6"/>
+      <selection activeCell="C6" sqref="C6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A4" s="33" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-    </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.15">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+    </row>
+    <row r="5" spans="1:12" ht="24" customHeight="1">
       <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
@@ -996,9 +1003,9 @@
       <c r="C5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="28" t="s">
         <v>4</v>
       </c>
@@ -1014,8 +1021,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.15">
-      <c r="A6" s="23"/>
+    <row r="6" spans="1:12" ht="48.75" customHeight="1">
+      <c r="A6" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="B6" s="24"/>
       <c r="C6" s="25" t="s">
         <v>8</v>
@@ -1027,10 +1036,10 @@
         <v>26</v>
       </c>
       <c r="H6" s="28"/>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="37"/>
+      <c r="J6" s="30"/>
       <c r="K6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1038,11 +1047,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12">
       <c r="A7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="31" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="21" t="s">
@@ -1072,9 +1081,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12">
       <c r="A8" s="22"/>
-      <c r="B8" s="30"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -1086,12 +1095,12 @@
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="25.5" customHeight="1">
       <c r="A9" s="2">
         <v>1</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="9"/>
@@ -1108,7 +1117,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="25.5" customHeight="1">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1124,7 +1133,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="25.5" customHeight="1">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1140,7 +1149,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="15.75">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1154,7 +1163,7 @@
       <c r="K12" s="8"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="42.75" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>24</v>
       </c>
@@ -1172,7 +1181,7 @@
       <c r="K13" s="15"/>
       <c r="L13" s="16"/>
     </row>
-    <row r="14" spans="1:12" ht="98" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="126" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="17"/>

</xml_diff>